<commit_message>
in all mj-devices: - seperated MJ8x8 clone - rev.5 - TCAN334 - poc.brd(generic) BOMs from device specific
</commit_message>
<xml_diff>
--- a/eagle design/mj514/BOM MJ514 - rev.1 - prod.xlsx
+++ b/eagle design/mj514/BOM MJ514 - rev.1 - prod.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$28</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$F$20</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="84">
   <si>
     <t>Qty</t>
   </si>
@@ -45,18 +45,12 @@
     <t>C0402</t>
   </si>
   <si>
-    <t>100k</t>
-  </si>
-  <si>
     <t>R-EU_R0402</t>
   </si>
   <si>
     <t>R0402</t>
   </si>
   <si>
-    <t>R201</t>
-  </si>
-  <si>
     <t>CPOL-EUE2.5-4V</t>
   </si>
   <si>
@@ -90,30 +84,12 @@
     <t>C802</t>
   </si>
   <si>
-    <t>47nF / 10V</t>
-  </si>
-  <si>
-    <t>C402</t>
-  </si>
-  <si>
     <t>4k7</t>
   </si>
   <si>
     <t>R1, R2</t>
   </si>
   <si>
-    <t>60R, 0.5W</t>
-  </si>
-  <si>
-    <t>R-EU_R0805</t>
-  </si>
-  <si>
-    <t>R0805</t>
-  </si>
-  <si>
-    <t>R402, R403</t>
-  </si>
-  <si>
     <t>C803</t>
   </si>
   <si>
@@ -156,18 +132,6 @@
     <t>IC901</t>
   </si>
   <si>
-    <t>LDK320AM33R</t>
-  </si>
-  <si>
-    <t>LDK320SOT-23-5L</t>
-  </si>
-  <si>
-    <t>SOT-23-5L</t>
-  </si>
-  <si>
-    <t>IC201</t>
-  </si>
-  <si>
     <t>LT1935ES5#TRMPBF</t>
   </si>
   <si>
@@ -204,18 +168,6 @@
     <t>D801</t>
   </si>
   <si>
-    <t>R3119N058A-TR-FE</t>
-  </si>
-  <si>
-    <t>R3119XXXA</t>
-  </si>
-  <si>
-    <t>SOT23-5</t>
-  </si>
-  <si>
-    <t>IC203</t>
-  </si>
-  <si>
     <t>SHT40-AD1F-R2</t>
   </si>
   <si>
@@ -228,48 +180,9 @@
     <t>IC501</t>
   </si>
   <si>
-    <t>STM32F042G6U6</t>
-  </si>
-  <si>
-    <t>STM32F042G6</t>
-  </si>
-  <si>
-    <t>UFQFPN-28</t>
-  </si>
-  <si>
-    <t>IC302</t>
-  </si>
-  <si>
-    <t>SZNUP2105LT1G</t>
-  </si>
-  <si>
-    <t>NUP2105L</t>
-  </si>
-  <si>
-    <t>SOT-23-3</t>
-  </si>
-  <si>
-    <t>IC402</t>
-  </si>
-  <si>
-    <t>TCAN334</t>
-  </si>
-  <si>
-    <t>CAN33X</t>
-  </si>
-  <si>
-    <t>SOT23-8</t>
-  </si>
-  <si>
-    <t>IC401</t>
-  </si>
-  <si>
     <t>0.1uF / 100V</t>
   </si>
   <si>
-    <t>C301, C305, C307, C405, C501, C902, C903, C904</t>
-  </si>
-  <si>
     <t>100uF / 25V</t>
   </si>
   <si>
@@ -288,9 +201,6 @@
     <t>C702, C801, C804</t>
   </si>
   <si>
-    <t>C201, C203, C204, C304, C701</t>
-  </si>
-  <si>
     <t>22nF / 50V</t>
   </si>
   <si>
@@ -315,9 +225,6 @@
     <t>C1608X5R1V475K080AC</t>
   </si>
   <si>
-    <t>603-AC0402JR-7W100KL</t>
-  </si>
-  <si>
     <t>603-AC0402JR-7W1KL</t>
   </si>
   <si>
@@ -336,24 +243,6 @@
     <t>80-C0402C223K5R7411</t>
   </si>
   <si>
-    <t>581-04025C473KAT2A</t>
-  </si>
-  <si>
-    <t>755-ESR10EZPD60R4</t>
-  </si>
-  <si>
-    <t>595-TCAN334GDCNT</t>
-  </si>
-  <si>
-    <t>511-STM32F042G6U6</t>
-  </si>
-  <si>
-    <t>511-LDK320AM33R</t>
-  </si>
-  <si>
-    <t>848-R3119N058A-TR-FE</t>
-  </si>
-  <si>
     <t>985-AS5601-ASOM</t>
   </si>
   <si>
@@ -372,9 +261,6 @@
     <t>863-MBRM120LT3G</t>
   </si>
   <si>
-    <t>863-SZNUP2105LT1G</t>
-  </si>
-  <si>
     <t>403-SHT40-AD1F-R2</t>
   </si>
   <si>
@@ -382,6 +268,12 @@
   </si>
   <si>
     <t>80-C0402C680K5R7867</t>
+  </si>
+  <si>
+    <t>C501, C902, C903, C904</t>
+  </si>
+  <si>
+    <t>C701</t>
   </si>
 </sst>
 </file>
@@ -720,10 +612,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="A20" sqref="A20:XFD20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -753,15 +645,15 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>92</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>80</v>
+        <v>52</v>
       </c>
       <c r="C2" t="s">
         <v>5</v>
@@ -770,10 +662,10 @@
         <v>6</v>
       </c>
       <c r="E2" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="F2" t="s">
-        <v>93</v>
+        <v>63</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -781,79 +673,79 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="F3" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="D4" t="s">
-        <v>12</v>
+        <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>13</v>
+        <v>54</v>
       </c>
       <c r="F4" t="s">
-        <v>118</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>55</v>
       </c>
       <c r="C5" t="s">
-        <v>8</v>
+        <v>56</v>
       </c>
       <c r="D5" t="s">
-        <v>9</v>
+        <v>57</v>
       </c>
       <c r="E5" t="s">
-        <v>83</v>
+        <v>58</v>
       </c>
       <c r="F5" t="s">
-        <v>99</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>84</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="D6" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>14</v>
       </c>
       <c r="F6" t="s">
-        <v>95</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -864,36 +756,36 @@
         <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="E7" t="s">
-        <v>16</v>
+        <v>83</v>
       </c>
       <c r="F7" t="s">
-        <v>98</v>
+        <v>64</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="B8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8" t="s">
+        <v>8</v>
+      </c>
+      <c r="E8" t="s">
         <v>17</v>
       </c>
-      <c r="C8" t="s">
-        <v>5</v>
-      </c>
-      <c r="D8" t="s">
-        <v>6</v>
-      </c>
-      <c r="E8" t="s">
-        <v>88</v>
-      </c>
       <c r="F8" t="s">
-        <v>94</v>
+        <v>69</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -901,19 +793,19 @@
         <v>1</v>
       </c>
       <c r="B9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C9" t="s">
+        <v>5</v>
+      </c>
+      <c r="D9" t="s">
+        <v>6</v>
+      </c>
+      <c r="E9" t="s">
         <v>18</v>
       </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-      <c r="D9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E9" t="s">
-        <v>19</v>
-      </c>
       <c r="F9" t="s">
-        <v>100</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -921,39 +813,39 @@
         <v>1</v>
       </c>
       <c r="B10" t="s">
-        <v>89</v>
+        <v>60</v>
       </c>
       <c r="C10" t="s">
-        <v>5</v>
+        <v>56</v>
       </c>
       <c r="D10" t="s">
-        <v>6</v>
+        <v>57</v>
       </c>
       <c r="E10" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>66</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>20</v>
       </c>
       <c r="C11" t="s">
-        <v>85</v>
+        <v>7</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>8</v>
       </c>
       <c r="E11" t="s">
         <v>21</v>
       </c>
       <c r="F11" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -961,7 +853,7 @@
         <v>1</v>
       </c>
       <c r="B12" t="s">
-        <v>22</v>
+        <v>61</v>
       </c>
       <c r="C12" t="s">
         <v>5</v>
@@ -970,50 +862,50 @@
         <v>6</v>
       </c>
       <c r="E12" t="s">
-        <v>23</v>
-      </c>
-      <c r="F12" t="s">
-        <v>104</v>
+        <v>22</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" t="s">
+        <v>8</v>
+      </c>
+      <c r="E13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
-        <v>8</v>
-      </c>
-      <c r="D13" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" t="s">
-        <v>25</v>
-      </c>
       <c r="F13" t="s">
-        <v>101</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
         <v>26</v>
       </c>
-      <c r="C14" t="s">
+      <c r="D14" t="s">
         <v>27</v>
       </c>
-      <c r="D14" t="s">
+      <c r="E14" t="s">
         <v>28</v>
       </c>
-      <c r="E14" t="s">
-        <v>29</v>
-      </c>
       <c r="F14" t="s">
-        <v>105</v>
+        <v>73</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1021,19 +913,19 @@
         <v>1</v>
       </c>
       <c r="B15" t="s">
-        <v>91</v>
+        <v>29</v>
       </c>
       <c r="C15" t="s">
-        <v>5</v>
-      </c>
-      <c r="D15" t="s">
-        <v>6</v>
+        <v>30</v>
+      </c>
+      <c r="D15">
+        <v>5050</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
-      </c>
-      <c r="F15" s="3" t="s">
-        <v>119</v>
+        <v>31</v>
+      </c>
+      <c r="F15" t="s">
+        <v>74</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -1041,19 +933,19 @@
         <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C16" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="D16" t="s">
-        <v>9</v>
+        <v>34</v>
       </c>
       <c r="E16" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="F16" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -1061,19 +953,19 @@
         <v>1</v>
       </c>
       <c r="B17" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="C17" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="D17" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="E17" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F17" t="s">
-        <v>110</v>
+        <v>76</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -1081,19 +973,19 @@
         <v>1</v>
       </c>
       <c r="B18" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="C18" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18">
-        <v>5050</v>
+        <v>41</v>
+      </c>
+      <c r="D18" t="s">
+        <v>42</v>
       </c>
       <c r="E18" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="F18" t="s">
-        <v>111</v>
+        <v>77</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -1101,19 +993,19 @@
         <v>1</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C19" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="D19" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="E19" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F19" t="s">
-        <v>112</v>
+        <v>78</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -1121,183 +1013,23 @@
         <v>1</v>
       </c>
       <c r="B20" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C20" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="D20" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="E20" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="F20" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1">
-        <v>1</v>
-      </c>
-      <c r="B21" t="s">
-        <v>48</v>
-      </c>
-      <c r="C21" t="s">
-        <v>49</v>
-      </c>
-      <c r="D21" t="s">
-        <v>50</v>
-      </c>
-      <c r="E21" t="s">
-        <v>51</v>
-      </c>
-      <c r="F21" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A22" s="1">
-        <v>1</v>
-      </c>
-      <c r="B22" t="s">
-        <v>52</v>
-      </c>
-      <c r="C22" t="s">
-        <v>53</v>
-      </c>
-      <c r="D22" t="s">
-        <v>54</v>
-      </c>
-      <c r="E22" t="s">
-        <v>55</v>
-      </c>
-      <c r="F22" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A23" s="1">
-        <v>1</v>
-      </c>
-      <c r="B23" t="s">
-        <v>56</v>
-      </c>
-      <c r="C23" t="s">
-        <v>57</v>
-      </c>
-      <c r="D23" t="s">
-        <v>58</v>
-      </c>
-      <c r="E23" t="s">
-        <v>59</v>
-      </c>
-      <c r="F23" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A24" s="1">
-        <v>1</v>
-      </c>
-      <c r="B24" t="s">
-        <v>60</v>
-      </c>
-      <c r="C24" t="s">
-        <v>61</v>
-      </c>
-      <c r="D24" t="s">
-        <v>62</v>
-      </c>
-      <c r="E24" t="s">
-        <v>63</v>
-      </c>
-      <c r="F24" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A25" s="1">
-        <v>1</v>
-      </c>
-      <c r="B25" t="s">
-        <v>64</v>
-      </c>
-      <c r="C25" t="s">
-        <v>65</v>
-      </c>
-      <c r="D25" t="s">
-        <v>66</v>
-      </c>
-      <c r="E25" t="s">
-        <v>67</v>
-      </c>
-      <c r="F25" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" s="1">
-        <v>1</v>
-      </c>
-      <c r="B26" t="s">
-        <v>68</v>
-      </c>
-      <c r="C26" t="s">
-        <v>69</v>
-      </c>
-      <c r="D26" t="s">
-        <v>70</v>
-      </c>
-      <c r="E26" t="s">
-        <v>71</v>
-      </c>
-      <c r="F26" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A27" s="1">
-        <v>1</v>
-      </c>
-      <c r="B27" t="s">
-        <v>72</v>
-      </c>
-      <c r="C27" t="s">
-        <v>73</v>
-      </c>
-      <c r="D27" t="s">
-        <v>74</v>
-      </c>
-      <c r="E27" t="s">
-        <v>75</v>
-      </c>
-      <c r="F27" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A28" s="1">
-        <v>1</v>
-      </c>
-      <c r="B28" t="s">
-        <v>76</v>
-      </c>
-      <c r="C28" t="s">
-        <v>77</v>
-      </c>
-      <c r="D28" t="s">
-        <v>78</v>
-      </c>
-      <c r="E28" t="s">
         <v>79</v>
       </c>
-      <c r="F28" t="s">
-        <v>106</v>
-      </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:F28"/>
+  <autoFilter ref="A1:F20"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="0"/>
 </worksheet>

</xml_diff>